<commit_message>
Update Modulos de actividades.xlsx
</commit_message>
<xml_diff>
--- a/Modulos de actividades.xlsx
+++ b/Modulos de actividades.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gabriel\Documents\GitHub\SAPDR\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="240" yWindow="60" windowWidth="20115" windowHeight="8010"/>
   </bookViews>
@@ -16,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="57">
   <si>
     <t>Modulos</t>
   </si>
@@ -57,9 +62,6 @@
     <t>pagina inicial do admin (painel de controlo) - admin</t>
   </si>
   <si>
-    <t>pagina inicial do site  - admin</t>
-  </si>
-  <si>
     <t>login do doente/representante - user</t>
   </si>
   <si>
@@ -87,9 +89,6 @@
     <t>relatorios - user</t>
   </si>
   <si>
-    <t>descricao do relatorio - user</t>
-  </si>
-  <si>
     <t>lista de  artigos - admin</t>
   </si>
   <si>
@@ -177,20 +176,29 @@
     <t>EP</t>
   </si>
   <si>
-    <t>GABRIEL</t>
-  </si>
-  <si>
     <t>EDMILSOM</t>
   </si>
   <si>
     <t>JOSSIAS</t>
+  </si>
+  <si>
+    <t>Enviar mensagens (contacte-nos) - USER</t>
+  </si>
+  <si>
+    <t>relatorios - userrelatorios - userrelatorios - user</t>
+  </si>
+  <si>
+    <t>pagina inicial do site  - user</t>
+  </si>
+  <si>
+    <t>PM</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -201,6 +209,14 @@
     <font>
       <b/>
       <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -248,21 +264,106 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="13">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF009900"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF009900"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF009900"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <border>
         <left style="thin">
@@ -288,12 +389,21 @@
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="Estilo de Tabela 1" pivot="0" count="1">
-      <tableStyleElement type="wholeTable" dxfId="0"/>
+      <tableStyleElement type="wholeTable" dxfId="12"/>
     </tableStyle>
   </tableStyles>
+  <colors>
+    <mruColors>
+      <color rgb="FF009900"/>
+      <color rgb="FF00FF00"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -302,7 +412,7 @@
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Escritório">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -340,9 +450,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Escritório">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -377,7 +487,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -412,7 +522,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Escritório">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -586,10 +696,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G37"/>
+  <dimension ref="A1:G38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -604,25 +714,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
     </row>
@@ -630,425 +740,534 @@
       <c r="A2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="E2" s="3" t="s">
+      <c r="C2" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2" t="s">
         <v>52</v>
-      </c>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>
-      <c r="B3" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3" t="s">
+      <c r="B3" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="E3" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3" t="s">
-        <v>51</v>
+      <c r="C3" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="4"/>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="F4" s="3"/>
-      <c r="G4" s="3" t="s">
-        <v>53</v>
-      </c>
+      <c r="C4" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="B5" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
-      <c r="G5" s="3"/>
+      <c r="C5" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="4"/>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
+      <c r="C6" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="4"/>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
+      <c r="C7" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="4"/>
-      <c r="B8" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="3"/>
+      <c r="B8" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
-      <c r="G9" s="3"/>
+        <v>16</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="4"/>
-      <c r="B10" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
-      <c r="G10" s="3"/>
+      <c r="B10" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="4"/>
-      <c r="B11" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="3"/>
-      <c r="G11" s="3"/>
+      <c r="B11" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="4"/>
-      <c r="B12" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
-      <c r="F12" s="3"/>
-      <c r="G12" s="3"/>
+      <c r="B12" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="2"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="4"/>
-      <c r="B13" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="C13" s="3"/>
-      <c r="D13" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="E13" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="F13" s="3"/>
-      <c r="G13" s="3"/>
+      <c r="B13" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="F13" s="2"/>
+      <c r="G13" s="2"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B14" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B14" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C14" s="3"/>
-      <c r="D14" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="E14" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="F14" s="3"/>
-      <c r="G14" s="3" t="s">
-        <v>54</v>
+      <c r="C14" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="F14" s="2"/>
+      <c r="G14" s="2" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="4"/>
-      <c r="B15" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="C15" s="3"/>
-      <c r="D15" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="E15" s="3"/>
-      <c r="F15" s="3"/>
-      <c r="G15" s="3"/>
+      <c r="B15" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
+      <c r="G15" s="2"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="4"/>
-      <c r="B16" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="C16" s="3"/>
-      <c r="D16" s="3"/>
-      <c r="E16" s="3"/>
-      <c r="F16" s="3"/>
-      <c r="G16" s="3"/>
+      <c r="B16" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="2"/>
+      <c r="G16" s="2"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="4"/>
-      <c r="B17" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="C17" s="3"/>
-      <c r="D17" s="3"/>
-      <c r="E17" s="3"/>
-      <c r="F17" s="3"/>
-      <c r="G17" s="3"/>
+      <c r="B17" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
+      <c r="F17" s="2"/>
+      <c r="G17" s="2"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C18" s="3"/>
-      <c r="D18" s="3"/>
-      <c r="E18" s="3"/>
-      <c r="F18" s="3"/>
-      <c r="G18" s="3"/>
+        <v>25</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="2"/>
+      <c r="G18" s="2"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="4"/>
-      <c r="B19" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="C19" s="3"/>
-      <c r="D19" s="3"/>
-      <c r="E19" s="3"/>
-      <c r="F19" s="3"/>
-      <c r="G19" s="3"/>
+      <c r="B19" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D19" s="2"/>
+      <c r="E19" s="2"/>
+      <c r="F19" s="2"/>
+      <c r="G19" s="2"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="4"/>
-      <c r="B20" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="C20" s="3"/>
-      <c r="D20" s="3"/>
-      <c r="E20" s="3"/>
-      <c r="F20" s="3"/>
-      <c r="G20" s="3"/>
+      <c r="B20" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D20" s="2"/>
+      <c r="E20" s="2"/>
+      <c r="F20" s="2"/>
+      <c r="G20" s="2"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="4"/>
-      <c r="B21" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="C21" s="3"/>
-      <c r="D21" s="3"/>
-      <c r="E21" s="3"/>
-      <c r="F21" s="3"/>
-      <c r="G21" s="3"/>
+      <c r="B21" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D21" s="2"/>
+      <c r="E21" s="2"/>
+      <c r="F21" s="2"/>
+      <c r="G21" s="2"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="B22" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="C22" s="3"/>
-      <c r="D22" s="3"/>
-      <c r="E22" s="3"/>
-      <c r="F22" s="3"/>
-      <c r="G22" s="3"/>
+        <v>26</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D22" s="2"/>
+      <c r="E22" s="2"/>
+      <c r="F22" s="2"/>
+      <c r="G22" s="2"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="4"/>
-      <c r="B23" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="C23" s="3"/>
-      <c r="D23" s="3"/>
-      <c r="E23" s="3"/>
-      <c r="F23" s="3"/>
-      <c r="G23" s="3"/>
+      <c r="B23" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D23" s="2"/>
+      <c r="E23" s="2"/>
+      <c r="F23" s="2"/>
+      <c r="G23" s="2"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="4"/>
-      <c r="B24" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="C24" s="3"/>
-      <c r="D24" s="3"/>
-      <c r="E24" s="3"/>
-      <c r="F24" s="3"/>
-      <c r="G24" s="3"/>
+      <c r="B24" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D24" s="2"/>
+      <c r="E24" s="2"/>
+      <c r="F24" s="2"/>
+      <c r="G24" s="2"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="B25" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="C25" s="3"/>
-      <c r="D25" s="3"/>
-      <c r="E25" s="3"/>
-      <c r="F25" s="3"/>
-      <c r="G25" s="3"/>
+        <v>29</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D25" s="2"/>
+      <c r="E25" s="2"/>
+      <c r="F25" s="2"/>
+      <c r="G25" s="2"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="4"/>
-      <c r="B26" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="C26" s="3"/>
-      <c r="D26" s="3"/>
-      <c r="E26" s="3"/>
-      <c r="F26" s="3"/>
-      <c r="G26" s="3"/>
+      <c r="B26" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D26" s="2"/>
+      <c r="E26" s="2"/>
+      <c r="F26" s="2"/>
+      <c r="G26" s="2"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="4"/>
-      <c r="B27" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="C27" s="3"/>
-      <c r="D27" s="3"/>
-      <c r="E27" s="3"/>
-      <c r="F27" s="3"/>
-      <c r="G27" s="3"/>
+      <c r="B27" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D27" s="2"/>
+      <c r="E27" s="2"/>
+      <c r="F27" s="2"/>
+      <c r="G27" s="2"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="4"/>
-      <c r="B28" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="C28" s="3"/>
-      <c r="D28" s="3"/>
-      <c r="E28" s="3"/>
-      <c r="F28" s="3"/>
-      <c r="G28" s="3"/>
+      <c r="B28" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D28" s="2"/>
+      <c r="E28" s="2"/>
+      <c r="F28" s="2"/>
+      <c r="G28" s="2"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="B29" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="C29" s="3"/>
-      <c r="D29" s="3"/>
-      <c r="E29" s="3"/>
-      <c r="F29" s="3"/>
-      <c r="G29" s="3"/>
+        <v>33</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D29" s="2"/>
+      <c r="E29" s="2"/>
+      <c r="F29" s="2"/>
+      <c r="G29" s="2"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="4"/>
-      <c r="B30" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="C30" s="3"/>
-      <c r="D30" s="3"/>
-      <c r="E30" s="3"/>
-      <c r="F30" s="3"/>
-      <c r="G30" s="3"/>
+      <c r="B30" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D30" s="2"/>
+      <c r="E30" s="2"/>
+      <c r="F30" s="2"/>
+      <c r="G30" s="2"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="4"/>
-      <c r="B31" s="3" t="s">
+      <c r="B31" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="E31" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="F31" s="2"/>
+      <c r="G31" s="2"/>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" s="4"/>
+      <c r="B32" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D32" s="2"/>
+      <c r="E32" s="2"/>
+      <c r="F32" s="2"/>
+      <c r="G32" s="2"/>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A33" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B33" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="C31" s="3"/>
-      <c r="D31" s="3"/>
-      <c r="E31" s="3"/>
-      <c r="F31" s="3"/>
-      <c r="G31" s="3"/>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A32" s="3" t="s">
+      <c r="C33" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D33" s="2"/>
+      <c r="E33" s="2"/>
+      <c r="F33" s="2"/>
+      <c r="G33" s="2"/>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A35" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="B32" s="3" t="s">
+      <c r="B35" s="3"/>
+      <c r="C35" s="3"/>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
         <v>39</v>
       </c>
-      <c r="C32" s="3"/>
-      <c r="D32" s="3"/>
-      <c r="E32" s="3"/>
-      <c r="F32" s="3"/>
-      <c r="G32" s="3"/>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" s="1" t="s">
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
         <v>40</v>
       </c>
-      <c r="B34" s="1"/>
-      <c r="C34" s="1"/>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
         <v>42</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>44</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="9">
-    <mergeCell ref="A34:C34"/>
+    <mergeCell ref="A2:A4"/>
+    <mergeCell ref="A5:A8"/>
+    <mergeCell ref="A9:A13"/>
+    <mergeCell ref="A35:C35"/>
     <mergeCell ref="A14:A17"/>
     <mergeCell ref="A18:A21"/>
     <mergeCell ref="A22:A24"/>
     <mergeCell ref="A25:A28"/>
-    <mergeCell ref="A29:A31"/>
-    <mergeCell ref="A2:A4"/>
-    <mergeCell ref="A5:A8"/>
-    <mergeCell ref="A9:A13"/>
+    <mergeCell ref="A29:A32"/>
   </mergeCells>
+  <conditionalFormatting sqref="E7">
+    <cfRule type="containsText" dxfId="5" priority="4" operator="containsText" text="F">
+      <formula>NOT(ISERROR(SEARCH("F",E7)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D7">
+    <cfRule type="cellIs" dxfId="4" priority="3" operator="equal">
+      <formula>"F"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A2:G33">
+    <cfRule type="cellIs" dxfId="3" priority="2" operator="equal">
+      <formula>"F"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A1:G33">
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
+      <formula>"EP"</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Update SAPDR Mockups - user -TIMBA.bmpr
</commit_message>
<xml_diff>
--- a/Modulos de actividades.xlsx
+++ b/Modulos de actividades.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="70">
   <si>
     <t>Modulos</t>
   </si>
@@ -228,6 +228,9 @@
   </si>
   <si>
     <t>Edmilson</t>
+  </si>
+  <si>
+    <t>f</t>
   </si>
 </sst>
 </file>
@@ -324,24 +327,24 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="1"/>
     <xf numFmtId="9" fontId="2" fillId="3" borderId="0" xfId="1" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Bom" xfId="1" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="15">
+  <dxfs count="7">
     <dxf>
       <fill>
         <patternFill>
@@ -388,62 +391,6 @@
       </fill>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <border>
         <left style="thin">
           <color auto="1"/>
@@ -468,7 +415,7 @@
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="Estilo de Tabela 1" pivot="0" count="1">
-      <tableStyleElement type="wholeTable" dxfId="14"/>
+      <tableStyleElement type="wholeTable" dxfId="6"/>
     </tableStyle>
   </tableStyles>
   <colors>
@@ -777,8 +724,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="J35" sqref="J35"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="G29" sqref="G29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -816,7 +763,7 @@
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="9" t="s">
         <v>6</v>
       </c>
       <c r="B2" s="2" t="s">
@@ -831,7 +778,7 @@
       <c r="G2" s="2"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="4"/>
+      <c r="A3" s="9"/>
       <c r="B3" s="2" t="s">
         <v>41</v>
       </c>
@@ -848,7 +795,7 @@
       <c r="G3" s="2"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="4"/>
+      <c r="A4" s="9"/>
       <c r="B4" s="2" t="s">
         <v>9</v>
       </c>
@@ -865,7 +812,7 @@
       <c r="G4" s="2"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="9" t="s">
         <v>15</v>
       </c>
       <c r="B5" s="2" t="s">
@@ -882,7 +829,7 @@
       <c r="G5" s="2"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="4"/>
+      <c r="A6" s="9"/>
       <c r="B6" s="2" t="s">
         <v>12</v>
       </c>
@@ -897,7 +844,7 @@
       <c r="G6" s="2"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="4"/>
+      <c r="A7" s="9"/>
       <c r="B7" s="2" t="s">
         <v>10</v>
       </c>
@@ -910,7 +857,7 @@
       <c r="G7" s="2"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="4"/>
+      <c r="A8" s="9"/>
       <c r="B8" s="2" t="s">
         <v>42</v>
       </c>
@@ -929,7 +876,7 @@
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
+      <c r="A9" s="9" t="s">
         <v>16</v>
       </c>
       <c r="B9" s="2" t="s">
@@ -939,14 +886,14 @@
       <c r="D9" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="E9" s="5" t="s">
+      <c r="E9" s="3" t="s">
         <v>53</v>
       </c>
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="4"/>
+      <c r="A10" s="9"/>
       <c r="B10" s="2" t="s">
         <v>13</v>
       </c>
@@ -963,7 +910,7 @@
       <c r="G10" s="2"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="4"/>
+      <c r="A11" s="9"/>
       <c r="B11" s="2" t="s">
         <v>17</v>
       </c>
@@ -976,7 +923,7 @@
       <c r="G11" s="2"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="4"/>
+      <c r="A12" s="9"/>
       <c r="B12" s="2" t="s">
         <v>14</v>
       </c>
@@ -984,7 +931,7 @@
         <v>62</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>48</v>
+        <v>69</v>
       </c>
       <c r="E12" s="2" t="s">
         <v>54</v>
@@ -995,8 +942,8 @@
       </c>
     </row>
     <row r="13" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="4"/>
-      <c r="B13" s="6" t="s">
+      <c r="A13" s="9"/>
+      <c r="B13" s="4" t="s">
         <v>57</v>
       </c>
       <c r="C13" s="2" t="s">
@@ -1010,7 +957,7 @@
       <c r="G13" s="2"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="4"/>
+      <c r="A14" s="9"/>
       <c r="B14" s="2" t="s">
         <v>43</v>
       </c>
@@ -1027,7 +974,7 @@
       <c r="G14" s="2"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="4" t="s">
+      <c r="A15" s="9" t="s">
         <v>18</v>
       </c>
       <c r="B15" s="2" t="s">
@@ -1046,7 +993,7 @@
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="4"/>
+      <c r="A16" s="9"/>
       <c r="B16" s="2" t="s">
         <v>20</v>
       </c>
@@ -1059,7 +1006,7 @@
       <c r="G16" s="2"/>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17" s="4"/>
+      <c r="A17" s="9"/>
       <c r="B17" s="2" t="s">
         <v>21</v>
       </c>
@@ -1072,7 +1019,7 @@
       <c r="G17" s="2"/>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A18" s="4" t="s">
+      <c r="A18" s="9" t="s">
         <v>24</v>
       </c>
       <c r="B18" s="2" t="s">
@@ -1080,7 +1027,7 @@
       </c>
       <c r="C18" s="2"/>
       <c r="D18" s="2" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="E18" s="2"/>
       <c r="F18" s="2"/>
@@ -1089,7 +1036,7 @@
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A19" s="4"/>
+      <c r="A19" s="9"/>
       <c r="B19" s="2" t="s">
         <v>44</v>
       </c>
@@ -1102,7 +1049,7 @@
       <c r="G19" s="2"/>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A20" s="4"/>
+      <c r="A20" s="9"/>
       <c r="B20" s="2" t="s">
         <v>23</v>
       </c>
@@ -1115,7 +1062,7 @@
       <c r="G20" s="2"/>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A21" s="4" t="s">
+      <c r="A21" s="9" t="s">
         <v>25</v>
       </c>
       <c r="B21" s="2" t="s">
@@ -1123,7 +1070,7 @@
       </c>
       <c r="C21" s="2"/>
       <c r="D21" s="2" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="E21" s="2"/>
       <c r="F21" s="2"/>
@@ -1132,13 +1079,13 @@
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A22" s="4"/>
+      <c r="A22" s="9"/>
       <c r="B22" s="2" t="s">
         <v>45</v>
       </c>
       <c r="C22" s="2"/>
       <c r="D22" s="2" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="E22" s="2"/>
       <c r="F22" s="2"/>
@@ -1147,22 +1094,24 @@
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A23" s="4"/>
+      <c r="A23" s="9"/>
       <c r="B23" s="2" t="s">
         <v>27</v>
       </c>
       <c r="C23" s="2"/>
       <c r="D23" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E23" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="E23" s="2"/>
       <c r="F23" s="2"/>
       <c r="G23" s="2" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A24" s="4" t="s">
+      <c r="A24" s="9" t="s">
         <v>28</v>
       </c>
       <c r="B24" s="2" t="s">
@@ -1173,10 +1122,10 @@
       <c r="E24" s="2"/>
       <c r="F24" s="2"/>
       <c r="G24" s="2"/>
-      <c r="K24" s="10"/>
+      <c r="K24" s="8"/>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A25" s="4"/>
+      <c r="A25" s="9"/>
       <c r="B25" s="2" t="s">
         <v>46</v>
       </c>
@@ -1191,7 +1140,7 @@
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A26" s="4"/>
+      <c r="A26" s="9"/>
       <c r="B26" s="2" t="s">
         <v>30</v>
       </c>
@@ -1204,7 +1153,7 @@
       <c r="G26" s="2"/>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A27" s="4" t="s">
+      <c r="A27" s="9" t="s">
         <v>32</v>
       </c>
       <c r="B27" s="2" t="s">
@@ -1219,7 +1168,7 @@
       <c r="G27" s="2"/>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A28" s="4"/>
+      <c r="A28" s="9"/>
       <c r="B28" s="2" t="s">
         <v>33</v>
       </c>
@@ -1232,7 +1181,7 @@
       <c r="G28" s="2"/>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A29" s="4"/>
+      <c r="A29" s="9"/>
       <c r="B29" s="2" t="s">
         <v>51</v>
       </c>
@@ -1262,40 +1211,40 @@
       <c r="G30" s="2"/>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A31" s="7"/>
-      <c r="B31" s="7"/>
-      <c r="C31" s="7"/>
-      <c r="D31" s="7"/>
-      <c r="E31" s="7"/>
-      <c r="F31" s="7"/>
-      <c r="G31" s="7"/>
+      <c r="A31" s="5"/>
+      <c r="B31" s="5"/>
+      <c r="C31" s="5"/>
+      <c r="D31" s="5"/>
+      <c r="E31" s="5"/>
+      <c r="F31" s="5"/>
+      <c r="G31" s="5"/>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A32" s="8" t="s">
+      <c r="A32" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="B32" s="8"/>
-      <c r="C32" s="8"/>
-      <c r="D32" s="9">
+      <c r="B32" s="6"/>
+      <c r="C32" s="6"/>
+      <c r="D32" s="7">
         <f>(COUNTIF(D2:D30,"F")/(COUNTA(D2:D30)+COUNTBLANK(D2:D30)))</f>
-        <v>0.72413793103448276</v>
-      </c>
-      <c r="E32" s="9">
+        <v>0.89655172413793105</v>
+      </c>
+      <c r="E32" s="7">
         <f>(COUNTIF(E2:E30,"F")/(COUNTA(E2:E30)+COUNTBLANK(E2:E30)))</f>
         <v>0.20689655172413793</v>
       </c>
-      <c r="F32" s="9">
+      <c r="F32" s="7">
         <f>(COUNTIF(F2:F30,"F")/(COUNTA(F2:F30)+COUNTBLANK(F2:F30)))</f>
         <v>0</v>
       </c>
-      <c r="G32" s="9"/>
+      <c r="G32" s="7"/>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" s="3" t="s">
+      <c r="A33" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="B33" s="3"/>
-      <c r="C33" s="3"/>
+      <c r="B33" s="10"/>
+      <c r="C33" s="10"/>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">

</xml_diff>

<commit_message>
Atribuicao de tarefa no modulo
Reservei uma tarefa que ja havia iniciado antes de termos o modulo.
</commit_message>
<xml_diff>
--- a/Modulos de actividades.xlsx
+++ b/Modulos de actividades.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gabriel\Documents\GitHub\SAPDR\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="240" yWindow="60" windowWidth="20115" windowHeight="8010"/>
   </bookViews>
@@ -16,12 +11,12 @@
     <sheet name="back-end" sheetId="2" r:id="rId2"/>
     <sheet name="base de dados" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="70">
   <si>
     <t>Modulos</t>
   </si>
@@ -170,9 +165,6 @@
     <t>EP</t>
   </si>
   <si>
-    <t>EDMILSOM</t>
-  </si>
-  <si>
     <t>JOSSIAS</t>
   </si>
   <si>
@@ -231,6 +223,9 @@
   </si>
   <si>
     <t>f</t>
+  </si>
+  <si>
+    <t>EDMILSON</t>
   </si>
 </sst>
 </file>
@@ -323,7 +318,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -339,9 +334,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Bom" xfId="1" builtinId="26"/>
+    <cellStyle name="Correcto" xfId="1" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="7">
@@ -438,7 +434,7 @@
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
   <a:themeElements>
-    <a:clrScheme name="Escritório">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -476,9 +472,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Escritório">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -513,7 +509,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -548,7 +544,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Escritório">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -725,7 +721,7 @@
   <dimension ref="A1:K37"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="G29" sqref="G29"/>
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -783,7 +779,7 @@
         <v>41</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>39</v>
@@ -800,7 +796,7 @@
         <v>9</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>39</v>
@@ -862,7 +858,7 @@
         <v>42</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>39</v>
@@ -880,14 +876,14 @@
         <v>16</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C9" s="2"/>
       <c r="D9" s="2" t="s">
         <v>39</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
@@ -898,7 +894,7 @@
         <v>13</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>39</v>
@@ -928,26 +924,26 @@
         <v>14</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F12" s="2"/>
       <c r="G12" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="9"/>
       <c r="B13" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="C13" s="2" t="s">
         <v>57</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>58</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>39</v>
@@ -962,13 +958,13 @@
         <v>43</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>39</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
@@ -989,7 +985,7 @@
       </c>
       <c r="F15" s="2"/>
       <c r="G15" s="2" t="s">
-        <v>49</v>
+        <v>69</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
@@ -1003,7 +999,9 @@
       </c>
       <c r="E16" s="2"/>
       <c r="F16" s="2"/>
-      <c r="G16" s="2"/>
+      <c r="G16" s="11" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="9"/>
@@ -1032,7 +1030,7 @@
       <c r="E18" s="2"/>
       <c r="F18" s="2"/>
       <c r="G18" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
@@ -1075,7 +1073,7 @@
       <c r="E21" s="2"/>
       <c r="F21" s="2"/>
       <c r="G21" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
@@ -1090,7 +1088,7 @@
       <c r="E22" s="2"/>
       <c r="F22" s="2"/>
       <c r="G22" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
@@ -1107,7 +1105,7 @@
       </c>
       <c r="F23" s="2"/>
       <c r="G23" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
@@ -1136,7 +1134,7 @@
       <c r="E25" s="2"/>
       <c r="F25" s="2"/>
       <c r="G25" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
@@ -1183,7 +1181,7 @@
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" s="9"/>
       <c r="B29" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C29" s="2"/>
       <c r="D29" s="2" t="s">
@@ -1203,7 +1201,7 @@
         <v>35</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D30" s="2"/>
       <c r="E30" s="2"/>
@@ -1221,7 +1219,7 @@
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B32" s="6"/>
       <c r="C32" s="6"/>
@@ -1263,7 +1261,7 @@
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
cabecalho, footer, paina para pedir apoio
</commit_message>
<xml_diff>
--- a/Modulos de actividades.xlsx
+++ b/Modulos de actividades.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="67">
   <si>
     <t>Modulos</t>
   </si>
@@ -165,9 +165,6 @@
     <t>EP</t>
   </si>
   <si>
-    <t>JOSSIAS</t>
-  </si>
-  <si>
     <t>Enviar mensagens (contacte-nos) - USER</t>
   </si>
   <si>
@@ -177,9 +174,6 @@
     <t>PM</t>
   </si>
   <si>
-    <t>U</t>
-  </si>
-  <si>
     <t>U-URGENTE</t>
   </si>
   <si>
@@ -214,9 +208,6 @@
   </si>
   <si>
     <t>Neima</t>
-  </si>
-  <si>
-    <t>Jossias</t>
   </si>
   <si>
     <t>Edmilson</t>
@@ -328,13 +319,13 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="1"/>
     <xf numFmtId="9" fontId="2" fillId="3" borderId="0" xfId="1" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Correcto" xfId="1" builtinId="26"/>
@@ -720,8 +711,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -759,7 +750,7 @@
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="9" t="s">
+      <c r="A2" s="10" t="s">
         <v>6</v>
       </c>
       <c r="B2" s="2" t="s">
@@ -774,12 +765,12 @@
       <c r="G2" s="2"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="9"/>
+      <c r="A3" s="10"/>
       <c r="B3" s="2" t="s">
         <v>41</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>39</v>
@@ -791,12 +782,12 @@
       <c r="G3" s="2"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="9"/>
+      <c r="A4" s="10"/>
       <c r="B4" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>39</v>
@@ -808,7 +799,7 @@
       <c r="G4" s="2"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="9" t="s">
+      <c r="A5" s="10" t="s">
         <v>15</v>
       </c>
       <c r="B5" s="2" t="s">
@@ -825,7 +816,7 @@
       <c r="G5" s="2"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="9"/>
+      <c r="A6" s="10"/>
       <c r="B6" s="2" t="s">
         <v>12</v>
       </c>
@@ -840,7 +831,7 @@
       <c r="G6" s="2"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="9"/>
+      <c r="A7" s="10"/>
       <c r="B7" s="2" t="s">
         <v>10</v>
       </c>
@@ -853,12 +844,12 @@
       <c r="G7" s="2"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="9"/>
+      <c r="A8" s="10"/>
       <c r="B8" s="2" t="s">
         <v>42</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>39</v>
@@ -872,29 +863,29 @@
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="9" t="s">
+      <c r="A9" s="10" t="s">
         <v>16</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C9" s="2"/>
       <c r="D9" s="2" t="s">
         <v>39</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>52</v>
+        <v>39</v>
       </c>
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="9"/>
+      <c r="A10" s="10"/>
       <c r="B10" s="2" t="s">
         <v>13</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>39</v>
@@ -906,7 +897,7 @@
       <c r="G10" s="2"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="9"/>
+      <c r="A11" s="10"/>
       <c r="B11" s="2" t="s">
         <v>17</v>
       </c>
@@ -919,31 +910,29 @@
       <c r="G11" s="2"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="9"/>
+      <c r="A12" s="10"/>
       <c r="B12" s="2" t="s">
         <v>14</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>53</v>
+        <v>39</v>
       </c>
       <c r="F12" s="2"/>
-      <c r="G12" s="2" t="s">
-        <v>66</v>
-      </c>
+      <c r="G12" s="2"/>
     </row>
     <row r="13" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="9"/>
+      <c r="A13" s="10"/>
       <c r="B13" s="4" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>39</v>
@@ -953,24 +942,24 @@
       <c r="G13" s="2"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="9"/>
+      <c r="A14" s="10"/>
       <c r="B14" s="2" t="s">
         <v>43</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>39</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="9" t="s">
+      <c r="A15" s="10" t="s">
         <v>18</v>
       </c>
       <c r="B15" s="2" t="s">
@@ -985,11 +974,11 @@
       </c>
       <c r="F15" s="2"/>
       <c r="G15" s="2" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="9"/>
+      <c r="A16" s="10"/>
       <c r="B16" s="2" t="s">
         <v>20</v>
       </c>
@@ -999,12 +988,12 @@
       </c>
       <c r="E16" s="2"/>
       <c r="F16" s="2"/>
-      <c r="G16" s="11" t="s">
-        <v>69</v>
+      <c r="G16" s="9" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17" s="9"/>
+      <c r="A17" s="10"/>
       <c r="B17" s="2" t="s">
         <v>21</v>
       </c>
@@ -1017,7 +1006,7 @@
       <c r="G17" s="2"/>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A18" s="9" t="s">
+      <c r="A18" s="10" t="s">
         <v>24</v>
       </c>
       <c r="B18" s="2" t="s">
@@ -1030,11 +1019,11 @@
       <c r="E18" s="2"/>
       <c r="F18" s="2"/>
       <c r="G18" s="2" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A19" s="9"/>
+      <c r="A19" s="10"/>
       <c r="B19" s="2" t="s">
         <v>44</v>
       </c>
@@ -1047,7 +1036,7 @@
       <c r="G19" s="2"/>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A20" s="9"/>
+      <c r="A20" s="10"/>
       <c r="B20" s="2" t="s">
         <v>23</v>
       </c>
@@ -1060,7 +1049,7 @@
       <c r="G20" s="2"/>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A21" s="9" t="s">
+      <c r="A21" s="10" t="s">
         <v>25</v>
       </c>
       <c r="B21" s="2" t="s">
@@ -1073,11 +1062,11 @@
       <c r="E21" s="2"/>
       <c r="F21" s="2"/>
       <c r="G21" s="2" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A22" s="9"/>
+      <c r="A22" s="10"/>
       <c r="B22" s="2" t="s">
         <v>45</v>
       </c>
@@ -1088,11 +1077,11 @@
       <c r="E22" s="2"/>
       <c r="F22" s="2"/>
       <c r="G22" s="2" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A23" s="9"/>
+      <c r="A23" s="10"/>
       <c r="B23" s="2" t="s">
         <v>27</v>
       </c>
@@ -1100,16 +1089,12 @@
       <c r="D23" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="E23" s="2" t="s">
-        <v>48</v>
-      </c>
+      <c r="E23" s="2"/>
       <c r="F23" s="2"/>
-      <c r="G23" s="2" t="s">
-        <v>49</v>
-      </c>
+      <c r="G23" s="2"/>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A24" s="9" t="s">
+      <c r="A24" s="10" t="s">
         <v>28</v>
       </c>
       <c r="B24" s="2" t="s">
@@ -1123,7 +1108,7 @@
       <c r="K24" s="8"/>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A25" s="9"/>
+      <c r="A25" s="10"/>
       <c r="B25" s="2" t="s">
         <v>46</v>
       </c>
@@ -1134,11 +1119,11 @@
       <c r="E25" s="2"/>
       <c r="F25" s="2"/>
       <c r="G25" s="2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A26" s="9"/>
+      <c r="A26" s="10"/>
       <c r="B26" s="2" t="s">
         <v>30</v>
       </c>
@@ -1151,7 +1136,7 @@
       <c r="G26" s="2"/>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A27" s="9" t="s">
+      <c r="A27" s="10" t="s">
         <v>32</v>
       </c>
       <c r="B27" s="2" t="s">
@@ -1166,7 +1151,7 @@
       <c r="G27" s="2"/>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A28" s="9"/>
+      <c r="A28" s="10"/>
       <c r="B28" s="2" t="s">
         <v>33</v>
       </c>
@@ -1179,9 +1164,9 @@
       <c r="G28" s="2"/>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A29" s="9"/>
+      <c r="A29" s="10"/>
       <c r="B29" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C29" s="2"/>
       <c r="D29" s="2" t="s">
@@ -1201,7 +1186,7 @@
         <v>35</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D30" s="2"/>
       <c r="E30" s="2"/>
@@ -1219,7 +1204,7 @@
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="6" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B32" s="6"/>
       <c r="C32" s="6"/>
@@ -1229,7 +1214,7 @@
       </c>
       <c r="E32" s="7">
         <f>(COUNTIF(E2:E30,"F")/(COUNTA(E2:E30)+COUNTBLANK(E2:E30)))</f>
-        <v>0.20689655172413793</v>
+        <v>0.27586206896551724</v>
       </c>
       <c r="F32" s="7">
         <f>(COUNTIF(F2:F30,"F")/(COUNTA(F2:F30)+COUNTBLANK(F2:F30)))</f>
@@ -1238,11 +1223,11 @@
       <c r="G32" s="7"/>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" s="10" t="s">
+      <c r="A33" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="B33" s="10"/>
-      <c r="C33" s="10"/>
+      <c r="B33" s="11"/>
+      <c r="C33" s="11"/>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
@@ -1261,7 +1246,7 @@
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
doencas raras actualisado e moolos de actividades
</commit_message>
<xml_diff>
--- a/Modulos de actividades.xlsx
+++ b/Modulos de actividades.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="60" windowWidth="20115" windowHeight="8010" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="60" windowWidth="20115" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="front-end" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="90">
   <si>
     <t>Modulos</t>
   </si>
@@ -284,6 +284,9 @@
   </si>
   <si>
     <t>PROGRESSO</t>
+  </si>
+  <si>
+    <t>JOSSIAS</t>
   </si>
 </sst>
 </file>
@@ -828,8 +831,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K39"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -914,10 +917,12 @@
         <v>39</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
+      <c r="G4" s="2" t="s">
+        <v>89</v>
+      </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="11" t="s">
@@ -1336,7 +1341,7 @@
       </c>
       <c r="E32" s="10">
         <f>(COUNTIF(E2:E30,"F")/(COUNTA(E2:E30)+COUNTBLANK(E2:E30)))</f>
-        <v>0.31034482758620691</v>
+        <v>0.27586206896551724</v>
       </c>
       <c r="F32" s="10">
         <f>(COUNTIF(F2:F30,"F")/(COUNTA(F2:F30)+COUNTBLANK(F2:F30)))</f>
@@ -1485,7 +1490,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:C13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
relattorios actualisados no user
</commit_message>
<xml_diff>
--- a/Modulos de actividades.xlsx
+++ b/Modulos de actividades.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\SAPDR\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="60" windowWidth="20115" windowHeight="8010" activeTab="3"/>
+    <workbookView xWindow="240" yWindow="60" windowWidth="20115" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="front-end" sheetId="1" r:id="rId1"/>
@@ -17,12 +12,12 @@
     <sheet name="base de dados" sheetId="3" r:id="rId3"/>
     <sheet name="ES" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="98">
   <si>
     <t>Modulos</t>
   </si>
@@ -496,7 +491,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Bom" xfId="1" builtinId="26"/>
+    <cellStyle name="Correcto" xfId="1" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="40">
@@ -824,7 +819,7 @@
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
   <a:themeElements>
-    <a:clrScheme name="Escritório">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -862,9 +857,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Escritório">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -899,7 +894,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -934,7 +929,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Escritório">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1110,8 +1105,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K40"/>
   <sheetViews>
-    <sheetView topLeftCell="B11" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+    <sheetView topLeftCell="B18" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1718,7 +1713,6 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="F1gx5rhJCmNzH92EP+Z3KPD+crNo2PmNTXEZwhtqn5f3pjErnqSVSfHZJEj2bnn7omrkVfIJ0bsE4KPZFzDQLg==" saltValue="XDw6ueb4rdIgRe0Nkys9sQ==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="9">
     <mergeCell ref="A2:A4"/>
     <mergeCell ref="A5:A8"/>
@@ -1812,8 +1806,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:F34"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E36" sqref="E36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2036,11 +2030,9 @@
         <v>23</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="E23" s="2" t="s">
-        <v>89</v>
-      </c>
+        <v>84</v>
+      </c>
+      <c r="E23" s="2"/>
     </row>
     <row r="24" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B24" s="22" t="s">
@@ -2074,11 +2066,9 @@
         <v>27</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="E26" s="2" t="s">
-        <v>89</v>
-      </c>
+        <v>84</v>
+      </c>
+      <c r="E26" s="2"/>
     </row>
     <row r="27" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B27" s="22" t="s">
@@ -2159,11 +2149,10 @@
       <c r="C34" s="8"/>
       <c r="D34" s="10">
         <f>(COUNTIF(D2:D31,"F")/(COUNTA(D2:D31)+COUNTBLANK(D2:D31)))</f>
-        <v>0.36666666666666664</v>
+        <v>0.43333333333333335</v>
       </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="OV5JhxOACw1GImrZVjFZIo9r7ku4+Ei77FA4s385CJmJwGFAss11J6ocFe+anW7EZ8lb/D8k4/vBtuwdnUpncg==" saltValue="/HA4Fkxh5uv3sZDs1eOVoA==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="8">
     <mergeCell ref="B27:B29"/>
     <mergeCell ref="B30:B32"/>
@@ -2286,8 +2275,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
relatorios, rodape, login, perfil do doente, etc actualizado ,
</commit_message>
<xml_diff>
--- a/Modulos de actividades.xlsx
+++ b/Modulos de actividades.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="60" windowWidth="20115" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="60" windowWidth="20115" windowHeight="8010" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="front-end" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="100">
   <si>
     <t>Modulos</t>
   </si>
@@ -311,6 +311,12 @@
   </si>
   <si>
     <t>vania</t>
+  </si>
+  <si>
+    <t>recuperar senha</t>
+  </si>
+  <si>
+    <t>joss</t>
   </si>
 </sst>
 </file>
@@ -1103,10 +1109,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K40"/>
+  <dimension ref="A1:K41"/>
   <sheetViews>
-    <sheetView topLeftCell="B18" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1363,83 +1369,82 @@
       <c r="G14" s="2"/>
       <c r="H14" s="7"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="22"/>
-      <c r="B15" s="2" t="s">
+      <c r="B15" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="F15" s="2"/>
+      <c r="G15" s="2"/>
+      <c r="H15" s="7"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="22"/>
+      <c r="B16" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="C15" s="2" t="s">
+      <c r="C16" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="D15" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="F15" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="G15" s="15"/>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="22" t="s">
+      <c r="D16" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="G16" s="15"/>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="B17" s="2" t="s">
         <v>19</v>
-      </c>
-      <c r="C16" s="2"/>
-      <c r="D16" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="E16" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="F16" s="2"/>
-      <c r="G16" s="2"/>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17" s="22"/>
-      <c r="B17" s="2" t="s">
-        <v>20</v>
       </c>
       <c r="C17" s="2"/>
       <c r="D17" s="2" t="s">
         <v>39</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>87</v>
+        <v>39</v>
       </c>
       <c r="F17" s="2"/>
-      <c r="G17" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="J17" t="s">
-        <v>59</v>
-      </c>
+      <c r="G17" s="2"/>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="22"/>
       <c r="B18" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C18" s="2"/>
       <c r="D18" s="2" t="s">
         <v>39</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>39</v>
+        <v>87</v>
       </c>
       <c r="F18" s="2"/>
-      <c r="G18" s="2"/>
+      <c r="G18" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="J18" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A19" s="22" t="s">
-        <v>24</v>
-      </c>
+      <c r="A19" s="22"/>
       <c r="B19" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C19" s="2"/>
       <c r="D19" s="2" t="s">
@@ -1452,15 +1457,17 @@
       <c r="G19" s="2"/>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A20" s="22"/>
+      <c r="A20" s="22" t="s">
+        <v>24</v>
+      </c>
       <c r="B20" s="2" t="s">
-        <v>44</v>
+        <v>22</v>
       </c>
       <c r="C20" s="2"/>
       <c r="D20" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="E20" s="15" t="s">
+      <c r="E20" s="2" t="s">
         <v>39</v>
       </c>
       <c r="F20" s="2"/>
@@ -1469,24 +1476,22 @@
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="22"/>
       <c r="B21" s="2" t="s">
-        <v>23</v>
+        <v>44</v>
       </c>
       <c r="C21" s="2"/>
       <c r="D21" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="E21" s="2" t="s">
+      <c r="E21" s="15" t="s">
         <v>39</v>
       </c>
       <c r="F21" s="2"/>
       <c r="G21" s="2"/>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A22" s="22" t="s">
-        <v>25</v>
-      </c>
+      <c r="A22" s="22"/>
       <c r="B22" s="2" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C22" s="2"/>
       <c r="D22" s="2" t="s">
@@ -1499,13 +1504,13 @@
       <c r="G22" s="2"/>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A23" s="22"/>
+      <c r="A23" s="22" t="s">
+        <v>25</v>
+      </c>
       <c r="B23" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>64</v>
-      </c>
+        <v>26</v>
+      </c>
+      <c r="C23" s="2"/>
       <c r="D23" s="2" t="s">
         <v>39</v>
       </c>
@@ -1518,9 +1523,11 @@
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="22"/>
       <c r="B24" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C24" s="2"/>
+        <v>45</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>64</v>
+      </c>
       <c r="D24" s="2" t="s">
         <v>39</v>
       </c>
@@ -1531,29 +1538,28 @@
       <c r="G24" s="2"/>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A25" s="22" t="s">
-        <v>28</v>
-      </c>
+      <c r="A25" s="22"/>
       <c r="B25" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C25" s="2"/>
       <c r="D25" s="2" t="s">
         <v>39</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="F25" s="2"/>
       <c r="G25" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="K25" s="7"/>
+        <v>99</v>
+      </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A26" s="22"/>
+      <c r="A26" s="22" t="s">
+        <v>28</v>
+      </c>
       <c r="B26" s="2" t="s">
-        <v>46</v>
+        <v>29</v>
       </c>
       <c r="C26" s="2"/>
       <c r="D26" s="2" t="s">
@@ -1566,17 +1572,18 @@
       <c r="G26" s="2" t="s">
         <v>83</v>
       </c>
+      <c r="K26" s="7"/>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="22"/>
       <c r="B27" s="2" t="s">
-        <v>30</v>
+        <v>46</v>
       </c>
       <c r="C27" s="2"/>
       <c r="D27" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="E27" s="3" t="s">
+      <c r="E27" s="2" t="s">
         <v>82</v>
       </c>
       <c r="F27" s="2"/>
@@ -1585,43 +1592,45 @@
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A28" s="22" t="s">
-        <v>32</v>
-      </c>
+      <c r="A28" s="22"/>
       <c r="B28" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C28" s="2"/>
       <c r="D28" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="E28" s="2" t="s">
-        <v>87</v>
+      <c r="E28" s="3" t="s">
+        <v>82</v>
       </c>
       <c r="F28" s="2"/>
       <c r="G28" s="2" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A29" s="22"/>
+      <c r="A29" s="22" t="s">
+        <v>32</v>
+      </c>
       <c r="B29" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C29" s="2"/>
       <c r="D29" s="2" t="s">
         <v>39</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>39</v>
+        <v>87</v>
       </c>
       <c r="F29" s="2"/>
-      <c r="G29" s="2"/>
+      <c r="G29" s="2" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" s="22"/>
       <c r="B30" s="2" t="s">
-        <v>47</v>
+        <v>33</v>
       </c>
       <c r="C30" s="2"/>
       <c r="D30" s="2" t="s">
@@ -1634,95 +1643,111 @@
       <c r="G30" s="2"/>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A31" s="2" t="s">
-        <v>34</v>
-      </c>
+      <c r="A31" s="22"/>
       <c r="B31" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="C31" s="2" t="s">
-        <v>50</v>
-      </c>
+        <v>47</v>
+      </c>
+      <c r="C31" s="2"/>
       <c r="D31" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="E31" s="2"/>
+      <c r="E31" s="2" t="s">
+        <v>39</v>
+      </c>
       <c r="F31" s="2"/>
       <c r="G31" s="2"/>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A32" s="5"/>
-      <c r="B32" s="5"/>
-      <c r="C32" s="5"/>
-      <c r="D32" s="5"/>
-      <c r="E32" s="5"/>
-      <c r="F32" s="5"/>
-      <c r="G32" s="5"/>
-    </row>
-    <row r="33" spans="1:7" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="8" t="s">
+      <c r="A32" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E32" s="2"/>
+      <c r="F32" s="2"/>
+      <c r="G32" s="2"/>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A33" s="5"/>
+      <c r="B33" s="5"/>
+      <c r="C33" s="5"/>
+      <c r="D33" s="5"/>
+      <c r="E33" s="5"/>
+      <c r="F33" s="5"/>
+      <c r="G33" s="5"/>
+    </row>
+    <row r="34" spans="1:7" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="B33" s="8"/>
-      <c r="C33" s="8"/>
-      <c r="D33" s="10">
-        <f>(COUNTIF(D2:D31,"F")/(COUNTA(D2:D31)+COUNTBLANK(D2:D31)))</f>
+      <c r="B34" s="8"/>
+      <c r="C34" s="8"/>
+      <c r="D34" s="10">
+        <f>(COUNTIF(D2:D32,"F")/(COUNTA(D2:D32)+COUNTBLANK(D2:D32)))</f>
         <v>1</v>
       </c>
-      <c r="E33" s="10">
-        <f>(COUNTIF(E2:E31,"F")/(COUNTA(E2:E31)+COUNTBLANK(E2:E31)))</f>
-        <v>0.8</v>
-      </c>
-      <c r="F33" s="10">
-        <f>(COUNTIF(F2:F31,"F")/(COUNTA(F2:F31)+COUNTBLANK(F2:F31)))</f>
-        <v>6.6666666666666666E-2</v>
-      </c>
-      <c r="G33" s="10"/>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A34" s="23"/>
-      <c r="B34" s="23"/>
-      <c r="C34" s="23"/>
+      <c r="E34" s="10">
+        <f>(COUNTIF(E2:E32,"F")/(COUNTA(E2:E32)+COUNTBLANK(E2:E32)))</f>
+        <v>0.77419354838709675</v>
+      </c>
+      <c r="F34" s="10">
+        <f>(COUNTIF(F2:F32,"F")/(COUNTA(F2:F32)+COUNTBLANK(F2:F32)))</f>
+        <v>6.4516129032258063E-2</v>
+      </c>
+      <c r="G34" s="10"/>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B35" s="8" t="s">
+      <c r="A35" s="23"/>
+      <c r="B35" s="23"/>
+      <c r="C35" s="23"/>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B36" s="8" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B36" s="6"/>
-    </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B37" s="6" t="s">
-        <v>37</v>
-      </c>
+      <c r="B37" s="6"/>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B38" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B39" s="6" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B40" s="6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B41" s="6" t="s">
         <v>49</v>
       </c>
     </row>
   </sheetData>
+  <sheetProtection password="CC33" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="9">
     <mergeCell ref="A2:A4"/>
     <mergeCell ref="A5:A8"/>
-    <mergeCell ref="A9:A15"/>
-    <mergeCell ref="A34:C34"/>
-    <mergeCell ref="A16:A18"/>
-    <mergeCell ref="A19:A21"/>
-    <mergeCell ref="A22:A24"/>
-    <mergeCell ref="A25:A27"/>
-    <mergeCell ref="A28:A30"/>
+    <mergeCell ref="A9:A16"/>
+    <mergeCell ref="A35:C35"/>
+    <mergeCell ref="A17:A19"/>
+    <mergeCell ref="A20:A22"/>
+    <mergeCell ref="A23:A25"/>
+    <mergeCell ref="A26:A28"/>
+    <mergeCell ref="A29:A31"/>
   </mergeCells>
   <conditionalFormatting sqref="E7">
     <cfRule type="containsText" dxfId="38" priority="9" operator="containsText" text="F">
@@ -1734,27 +1759,27 @@
       <formula>"F"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A14 C14:G14 A15:G32 A2:G13">
+  <conditionalFormatting sqref="A14:A15 C14:G15 A16:G33 A2:G13">
     <cfRule type="cellIs" dxfId="36" priority="7" operator="equal">
       <formula>"F"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A14 C14:G14 A15:G32 A1:G13">
+  <conditionalFormatting sqref="A14:A15 C14:G15 A16:G33 A1:G13">
     <cfRule type="cellIs" dxfId="35" priority="6" operator="equal">
       <formula>"EP"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D37">
+  <conditionalFormatting sqref="D38">
     <cfRule type="cellIs" dxfId="34" priority="5" operator="equal">
       <formula>"U"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A14 C14:XFD14 A43:XFD1048576 A39:A42 C35:XFD42 B37:B40 A15:XFD34 A1:XFD13">
+  <conditionalFormatting sqref="A14:A15 C14:XFD15 A44:XFD1048576 A40:A43 C36:XFD43 B38:B41 A16:XFD35 A1:XFD13">
     <cfRule type="cellIs" dxfId="33" priority="4" operator="equal">
       <formula>"U"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G20">
+  <conditionalFormatting sqref="G21">
     <cfRule type="dataBar" priority="3">
       <dataBar>
         <cfvo type="min"/>
@@ -1768,12 +1793,12 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E29">
+  <conditionalFormatting sqref="E30">
     <cfRule type="cellIs" dxfId="32" priority="2" operator="equal">
       <formula>"PM"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A1:G31">
+  <conditionalFormatting sqref="A1:G32">
     <cfRule type="cellIs" dxfId="31" priority="1" operator="equal">
       <formula>"PM"</formula>
     </cfRule>
@@ -1794,7 +1819,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>G20</xm:sqref>
+          <xm:sqref>G21</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
@@ -1806,8 +1831,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:F34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E36" sqref="E36"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2153,6 +2178,7 @@
       </c>
     </row>
   </sheetData>
+  <sheetProtection password="CC33" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="8">
     <mergeCell ref="B27:B29"/>
     <mergeCell ref="B30:B32"/>
@@ -2212,8 +2238,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:C13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2259,13 +2285,14 @@
         <v>79</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>84</v>
+        <v>39</v>
       </c>
     </row>
     <row r="13" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C13" s="7"/>
     </row>
   </sheetData>
+  <sheetProtection password="CC33" sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
@@ -2276,7 +2303,7 @@
   <dimension ref="A1:H24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
revisao da interface - pedidos de apoio, instituicoes, etc
</commit_message>
<xml_diff>
--- a/Modulos de actividades.xlsx
+++ b/Modulos de actividades.xlsx
@@ -4,20 +4,21 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="60" windowWidth="20115" windowHeight="8010" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="60" windowWidth="20115" windowHeight="8010" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="front-end" sheetId="1" r:id="rId1"/>
     <sheet name="back-end" sheetId="2" r:id="rId2"/>
     <sheet name="base de dados" sheetId="3" r:id="rId3"/>
     <sheet name="ES" sheetId="4" r:id="rId4"/>
+    <sheet name="notas" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="107">
   <si>
     <t>Modulos</t>
   </si>
@@ -316,14 +317,35 @@
     <t>recuperar senha</t>
   </si>
   <si>
-    <t>joss</t>
+    <t>funcionalidade por adicionar/melhorar</t>
+  </si>
+  <si>
+    <t>filtros nas tabelas do admin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">editar tabela posts na bd </t>
+  </si>
+  <si>
+    <t>paginacao (campanhas, tabelas do admin)</t>
+  </si>
+  <si>
+    <t>perfil (visualisar e editar)</t>
+  </si>
+  <si>
+    <t>botoes de formularios em steps devem ser responsivos</t>
+  </si>
+  <si>
+    <t>todas tabelas de publicacoes devem ter data</t>
+  </si>
+  <si>
+    <t>Nas edicoes do admin o botao cancelar nao pode ser um  type="reset"</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -364,6 +386,12 @@
     <font>
       <sz val="16"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -448,7 +476,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -489,11 +517,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1109,10 +1138,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K41"/>
+  <dimension ref="A1:K43"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+    <sheetView topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1150,7 +1179,7 @@
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="22" t="s">
+      <c r="A2" s="24" t="s">
         <v>6</v>
       </c>
       <c r="B2" s="2" t="s">
@@ -1167,7 +1196,7 @@
       <c r="G2" s="2"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="22"/>
+      <c r="A3" s="24"/>
       <c r="B3" s="2" t="s">
         <v>41</v>
       </c>
@@ -1188,7 +1217,7 @@
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="22"/>
+      <c r="A4" s="24"/>
       <c r="B4" s="2" t="s">
         <v>9</v>
       </c>
@@ -1205,7 +1234,7 @@
       <c r="G4" s="2"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="22" t="s">
+      <c r="A5" s="24" t="s">
         <v>15</v>
       </c>
       <c r="B5" s="2" t="s">
@@ -1222,24 +1251,24 @@
       <c r="G5" s="2"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="22"/>
+      <c r="A6" s="24"/>
       <c r="B6" s="2" t="s">
-        <v>12</v>
+        <v>98</v>
       </c>
       <c r="C6" s="2"/>
       <c r="D6" s="2" t="s">
-        <v>39</v>
+        <v>84</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>39</v>
+        <v>84</v>
       </c>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="22"/>
+      <c r="A7" s="24"/>
       <c r="B7" s="2" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C7" s="2"/>
       <c r="D7" s="2" t="s">
@@ -1252,48 +1281,42 @@
       <c r="G7" s="2"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="22"/>
+      <c r="A8" s="24"/>
       <c r="B8" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>54</v>
-      </c>
+        <v>103</v>
+      </c>
+      <c r="C8" s="2"/>
       <c r="D8" s="2" t="s">
-        <v>39</v>
+        <v>84</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>84</v>
-      </c>
+        <v>84</v>
+      </c>
+      <c r="F8" s="2"/>
       <c r="G8" s="2"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="22" t="s">
-        <v>16</v>
-      </c>
+      <c r="A9" s="24"/>
       <c r="B9" s="2" t="s">
-        <v>48</v>
+        <v>10</v>
       </c>
       <c r="C9" s="2"/>
       <c r="D9" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="E9" s="3" t="s">
+      <c r="E9" s="2" t="s">
         <v>39</v>
       </c>
       <c r="F9" s="2"/>
-      <c r="G9" s="15"/>
+      <c r="G9" s="2"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="22"/>
+      <c r="A10" s="24"/>
       <c r="B10" s="2" t="s">
-        <v>13</v>
+        <v>42</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>39</v>
@@ -1301,30 +1324,36 @@
       <c r="E10" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="F10" s="2"/>
+      <c r="F10" s="2" t="s">
+        <v>84</v>
+      </c>
       <c r="G10" s="2"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="22"/>
+      <c r="A11" s="24" t="s">
+        <v>16</v>
+      </c>
       <c r="B11" s="2" t="s">
-        <v>17</v>
+        <v>48</v>
       </c>
       <c r="C11" s="2"/>
       <c r="D11" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="E11" s="2" t="s">
+      <c r="E11" s="3" t="s">
         <v>39</v>
       </c>
       <c r="F11" s="2"/>
-      <c r="G11" s="2"/>
+      <c r="G11" s="15"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="22"/>
+      <c r="A12" s="24"/>
       <c r="B12" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="C12" s="2"/>
+        <v>13</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>56</v>
+      </c>
       <c r="D12" s="2" t="s">
         <v>39</v>
       </c>
@@ -1335,13 +1364,11 @@
       <c r="G12" s="2"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="22"/>
+      <c r="A13" s="24"/>
       <c r="B13" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>55</v>
-      </c>
+        <v>17</v>
+      </c>
+      <c r="C13" s="2"/>
       <c r="D13" s="2" t="s">
         <v>39</v>
       </c>
@@ -1351,14 +1378,12 @@
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
     </row>
-    <row r="14" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A14" s="22"/>
-      <c r="B14" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>60</v>
-      </c>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="24"/>
+      <c r="B14" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C14" s="2"/>
       <c r="D14" s="2" t="s">
         <v>39</v>
       </c>
@@ -1367,31 +1392,31 @@
       </c>
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
-      <c r="H14" s="7"/>
-    </row>
-    <row r="15" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A15" s="22"/>
-      <c r="B15" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="C15" s="2"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="24"/>
+      <c r="B15" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>55</v>
+      </c>
       <c r="D15" s="2" t="s">
-        <v>84</v>
+        <v>39</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>84</v>
+        <v>39</v>
       </c>
       <c r="F15" s="2"/>
       <c r="G15" s="2"/>
-      <c r="H15" s="7"/>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="22"/>
-      <c r="B16" s="2" t="s">
-        <v>43</v>
+    </row>
+    <row r="16" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A16" s="24"/>
+      <c r="B16" s="4" t="s">
+        <v>51</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="D16" s="2" t="s">
         <v>39</v>
@@ -1399,52 +1424,51 @@
       <c r="E16" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="F16" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="G16" s="15"/>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17" s="22" t="s">
-        <v>18</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>19</v>
+      <c r="F16" s="2"/>
+      <c r="G16" s="2"/>
+      <c r="H16" s="7"/>
+    </row>
+    <row r="17" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A17" s="24"/>
+      <c r="B17" s="4" t="s">
+        <v>98</v>
       </c>
       <c r="C17" s="2"/>
       <c r="D17" s="2" t="s">
-        <v>39</v>
+        <v>84</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>39</v>
+        <v>84</v>
       </c>
       <c r="F17" s="2"/>
       <c r="G17" s="2"/>
+      <c r="H17" s="7"/>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A18" s="22"/>
+      <c r="A18" s="24"/>
       <c r="B18" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C18" s="2"/>
+        <v>43</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>57</v>
+      </c>
       <c r="D18" s="2" t="s">
         <v>39</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="F18" s="2"/>
-      <c r="G18" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="J18" t="s">
-        <v>59</v>
-      </c>
+        <v>39</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="G18" s="15"/>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A19" s="22"/>
+      <c r="A19" s="24" t="s">
+        <v>18</v>
+      </c>
       <c r="B19" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C19" s="2"/>
       <c r="D19" s="2" t="s">
@@ -1457,41 +1481,46 @@
       <c r="G19" s="2"/>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A20" s="22" t="s">
-        <v>24</v>
-      </c>
+      <c r="A20" s="24"/>
       <c r="B20" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C20" s="2"/>
       <c r="D20" s="2" t="s">
         <v>39</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>39</v>
+        <v>87</v>
       </c>
       <c r="F20" s="2"/>
-      <c r="G20" s="2"/>
+      <c r="G20" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="J20" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A21" s="22"/>
+      <c r="A21" s="24"/>
       <c r="B21" s="2" t="s">
-        <v>44</v>
+        <v>21</v>
       </c>
       <c r="C21" s="2"/>
       <c r="D21" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="E21" s="15" t="s">
+      <c r="E21" s="2" t="s">
         <v>39</v>
       </c>
       <c r="F21" s="2"/>
       <c r="G21" s="2"/>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A22" s="22"/>
+      <c r="A22" s="24" t="s">
+        <v>24</v>
+      </c>
       <c r="B22" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C22" s="2"/>
       <c r="D22" s="2" t="s">
@@ -1504,30 +1533,26 @@
       <c r="G22" s="2"/>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A23" s="22" t="s">
-        <v>25</v>
-      </c>
+      <c r="A23" s="24"/>
       <c r="B23" s="2" t="s">
-        <v>26</v>
+        <v>44</v>
       </c>
       <c r="C23" s="2"/>
       <c r="D23" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="E23" s="2" t="s">
+      <c r="E23" s="15" t="s">
         <v>39</v>
       </c>
       <c r="F23" s="2"/>
       <c r="G23" s="2"/>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A24" s="22"/>
+      <c r="A24" s="24"/>
       <c r="B24" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="C24" s="2" t="s">
-        <v>64</v>
-      </c>
+        <v>23</v>
+      </c>
+      <c r="C24" s="2"/>
       <c r="D24" s="2" t="s">
         <v>39</v>
       </c>
@@ -1538,248 +1563,279 @@
       <c r="G24" s="2"/>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A25" s="22"/>
+      <c r="A25" s="24" t="s">
+        <v>25</v>
+      </c>
       <c r="B25" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C25" s="2"/>
       <c r="D25" s="2" t="s">
         <v>39</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>87</v>
+        <v>39</v>
       </c>
       <c r="F25" s="2"/>
-      <c r="G25" s="2" t="s">
-        <v>99</v>
-      </c>
+      <c r="G25" s="2"/>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A26" s="22" t="s">
-        <v>28</v>
-      </c>
+      <c r="A26" s="24"/>
       <c r="B26" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C26" s="2"/>
+        <v>45</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>64</v>
+      </c>
       <c r="D26" s="2" t="s">
         <v>39</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>82</v>
+        <v>39</v>
       </c>
       <c r="F26" s="2"/>
-      <c r="G26" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="K26" s="7"/>
+      <c r="G26" s="2"/>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A27" s="22"/>
+      <c r="A27" s="24"/>
       <c r="B27" s="2" t="s">
-        <v>46</v>
+        <v>27</v>
       </c>
       <c r="C27" s="2"/>
       <c r="D27" s="2" t="s">
         <v>39</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="F27" s="2"/>
-      <c r="G27" s="2" t="s">
-        <v>83</v>
-      </c>
+      <c r="G27" s="2"/>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A28" s="22"/>
+      <c r="A28" s="24" t="s">
+        <v>28</v>
+      </c>
       <c r="B28" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C28" s="2"/>
       <c r="D28" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="E28" s="3" t="s">
+      <c r="E28" s="2" t="s">
         <v>82</v>
       </c>
       <c r="F28" s="2"/>
       <c r="G28" s="2" t="s">
         <v>83</v>
       </c>
+      <c r="K28" s="7"/>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A29" s="22" t="s">
-        <v>32</v>
-      </c>
+      <c r="A29" s="24"/>
       <c r="B29" s="2" t="s">
-        <v>31</v>
+        <v>46</v>
       </c>
       <c r="C29" s="2"/>
       <c r="D29" s="2" t="s">
         <v>39</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="F29" s="2"/>
       <c r="G29" s="2" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A30" s="22"/>
+      <c r="A30" s="24"/>
       <c r="B30" s="2" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C30" s="2"/>
       <c r="D30" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="E30" s="2" t="s">
-        <v>39</v>
+      <c r="E30" s="3" t="s">
+        <v>82</v>
       </c>
       <c r="F30" s="2"/>
-      <c r="G30" s="2"/>
+      <c r="G30" s="2" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A31" s="22"/>
+      <c r="A31" s="24" t="s">
+        <v>32</v>
+      </c>
       <c r="B31" s="2" t="s">
-        <v>47</v>
+        <v>31</v>
       </c>
       <c r="C31" s="2"/>
       <c r="D31" s="2" t="s">
         <v>39</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>39</v>
+        <v>87</v>
       </c>
       <c r="F31" s="2"/>
-      <c r="G31" s="2"/>
+      <c r="G31" s="2" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A32" s="2" t="s">
-        <v>34</v>
-      </c>
+      <c r="A32" s="24"/>
       <c r="B32" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="C32" s="2" t="s">
-        <v>50</v>
-      </c>
+        <v>33</v>
+      </c>
+      <c r="C32" s="2"/>
       <c r="D32" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="E32" s="2"/>
+      <c r="E32" s="2" t="s">
+        <v>39</v>
+      </c>
       <c r="F32" s="2"/>
       <c r="G32" s="2"/>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A33" s="5"/>
-      <c r="B33" s="5"/>
-      <c r="C33" s="5"/>
-      <c r="D33" s="5"/>
-      <c r="E33" s="5"/>
-      <c r="F33" s="5"/>
-      <c r="G33" s="5"/>
-    </row>
-    <row r="34" spans="1:7" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="8" t="s">
+      <c r="A33" s="24"/>
+      <c r="B33" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C33" s="2"/>
+      <c r="D33" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E33" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F33" s="2"/>
+      <c r="G33" s="2"/>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A34" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E34" s="2"/>
+      <c r="F34" s="2"/>
+      <c r="G34" s="2"/>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A35" s="5"/>
+      <c r="B35" s="5"/>
+      <c r="C35" s="5"/>
+      <c r="D35" s="5"/>
+      <c r="E35" s="5"/>
+      <c r="F35" s="5"/>
+      <c r="G35" s="5"/>
+    </row>
+    <row r="36" spans="1:7" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="B34" s="8"/>
-      <c r="C34" s="8"/>
-      <c r="D34" s="10">
-        <f>(COUNTIF(D2:D32,"F")/(COUNTA(D2:D32)+COUNTBLANK(D2:D32)))</f>
+      <c r="B36" s="8"/>
+      <c r="C36" s="8"/>
+      <c r="D36" s="10">
+        <f>(COUNTIF(D2:D34,"F")/(COUNTA(D2:D34)+COUNTBLANK(D2:D34)))</f>
         <v>1</v>
       </c>
-      <c r="E34" s="10">
-        <f>(COUNTIF(E2:E32,"F")/(COUNTA(E2:E32)+COUNTBLANK(E2:E32)))</f>
-        <v>0.77419354838709675</v>
-      </c>
-      <c r="F34" s="10">
-        <f>(COUNTIF(F2:F32,"F")/(COUNTA(F2:F32)+COUNTBLANK(F2:F32)))</f>
-        <v>6.4516129032258063E-2</v>
-      </c>
-      <c r="G34" s="10"/>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A35" s="23"/>
-      <c r="B35" s="23"/>
-      <c r="C35" s="23"/>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B36" s="8" t="s">
+      <c r="E36" s="10">
+        <f>(COUNTIF(E2:E34,"F")/(COUNTA(E2:E34)+COUNTBLANK(E2:E34)))</f>
+        <v>0.81818181818181823</v>
+      </c>
+      <c r="F36" s="10">
+        <f>(COUNTIF(F2:F34,"F")/(COUNTA(F2:F34)+COUNTBLANK(F2:F34)))</f>
+        <v>6.0606060606060608E-2</v>
+      </c>
+      <c r="G36" s="10"/>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A37" s="23"/>
+      <c r="B37" s="23"/>
+      <c r="C37" s="23"/>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B38" s="8" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B37" s="6"/>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B38" s="6" t="s">
-        <v>37</v>
-      </c>
-    </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B39" s="6" t="s">
-        <v>38</v>
-      </c>
+      <c r="B39" s="6"/>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B40" s="6" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B41" s="6" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B42" s="6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B43" s="6" t="s">
         <v>49</v>
       </c>
     </row>
   </sheetData>
-  <sheetProtection password="CC33" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="9">
+    <mergeCell ref="A37:C37"/>
     <mergeCell ref="A2:A4"/>
-    <mergeCell ref="A5:A8"/>
-    <mergeCell ref="A9:A16"/>
-    <mergeCell ref="A35:C35"/>
-    <mergeCell ref="A17:A19"/>
-    <mergeCell ref="A20:A22"/>
-    <mergeCell ref="A23:A25"/>
-    <mergeCell ref="A26:A28"/>
-    <mergeCell ref="A29:A31"/>
+    <mergeCell ref="A5:A10"/>
+    <mergeCell ref="A11:A18"/>
+    <mergeCell ref="A19:A21"/>
+    <mergeCell ref="A22:A24"/>
+    <mergeCell ref="A25:A27"/>
+    <mergeCell ref="A28:A30"/>
+    <mergeCell ref="A31:A33"/>
   </mergeCells>
-  <conditionalFormatting sqref="E7">
+  <conditionalFormatting sqref="E9">
     <cfRule type="containsText" dxfId="38" priority="9" operator="containsText" text="F">
-      <formula>NOT(ISERROR(SEARCH("F",E7)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D7">
+      <formula>NOT(ISERROR(SEARCH("F",E9)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D9">
     <cfRule type="cellIs" dxfId="37" priority="8" operator="equal">
       <formula>"F"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A14:A15 C14:G15 A16:G33 A2:G13">
+  <conditionalFormatting sqref="A16:A17 C16:G17 A18:G35 A2:G15">
     <cfRule type="cellIs" dxfId="36" priority="7" operator="equal">
       <formula>"F"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A14:A15 C14:G15 A16:G33 A1:G13">
+  <conditionalFormatting sqref="A16:A17 C16:G17 A18:G35 A1:G15">
     <cfRule type="cellIs" dxfId="35" priority="6" operator="equal">
       <formula>"EP"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D38">
+  <conditionalFormatting sqref="D40">
     <cfRule type="cellIs" dxfId="34" priority="5" operator="equal">
       <formula>"U"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A14:A15 C14:XFD15 A44:XFD1048576 A40:A43 C36:XFD43 B38:B41 A16:XFD35 A1:XFD13">
+  <conditionalFormatting sqref="A16:A17 C16:XFD17 A46:XFD1048576 A42:A45 C38:XFD45 B40:B43 A18:XFD37 A1:XFD15">
     <cfRule type="cellIs" dxfId="33" priority="4" operator="equal">
       <formula>"U"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G21">
+  <conditionalFormatting sqref="G23">
     <cfRule type="dataBar" priority="3">
       <dataBar>
         <cfvo type="min"/>
@@ -1793,12 +1849,12 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E30">
+  <conditionalFormatting sqref="E32">
     <cfRule type="cellIs" dxfId="32" priority="2" operator="equal">
       <formula>"PM"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A1:G32">
+  <conditionalFormatting sqref="A1:G34">
     <cfRule type="cellIs" dxfId="31" priority="1" operator="equal">
       <formula>"PM"</formula>
     </cfRule>
@@ -1819,7 +1875,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>G21</xm:sqref>
+          <xm:sqref>G23</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
@@ -1857,7 +1913,7 @@
       </c>
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B4" s="22" t="s">
+      <c r="B4" s="24" t="s">
         <v>6</v>
       </c>
       <c r="C4" s="2" t="s">
@@ -1869,7 +1925,7 @@
       <c r="E4" s="2"/>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B5" s="22"/>
+      <c r="B5" s="24"/>
       <c r="C5" s="2" t="s">
         <v>41</v>
       </c>
@@ -1879,7 +1935,7 @@
       <c r="E5" s="2"/>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B6" s="22"/>
+      <c r="B6" s="24"/>
       <c r="C6" s="2" t="s">
         <v>9</v>
       </c>
@@ -1889,7 +1945,7 @@
       <c r="E6" s="2"/>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B7" s="22" t="s">
+      <c r="B7" s="24" t="s">
         <v>15</v>
       </c>
       <c r="C7" s="2" t="s">
@@ -1901,7 +1957,7 @@
       <c r="E7" s="2"/>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B8" s="22"/>
+      <c r="B8" s="24"/>
       <c r="C8" s="2" t="s">
         <v>12</v>
       </c>
@@ -1909,7 +1965,7 @@
       <c r="E8" s="2"/>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B9" s="22"/>
+      <c r="B9" s="24"/>
       <c r="C9" s="2" t="s">
         <v>10</v>
       </c>
@@ -1920,7 +1976,7 @@
       <c r="F9" s="7"/>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B10" s="22"/>
+      <c r="B10" s="24"/>
       <c r="C10" s="2" t="s">
         <v>42</v>
       </c>
@@ -1928,7 +1984,7 @@
       <c r="E10" s="2"/>
     </row>
     <row r="11" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B11" s="22" t="s">
+      <c r="B11" s="24" t="s">
         <v>16</v>
       </c>
       <c r="C11" s="2" t="s">
@@ -1938,7 +1994,7 @@
       <c r="E11" s="2"/>
     </row>
     <row r="12" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B12" s="22"/>
+      <c r="B12" s="24"/>
       <c r="C12" s="2" t="s">
         <v>13</v>
       </c>
@@ -1948,7 +2004,7 @@
       <c r="E12" s="2"/>
     </row>
     <row r="13" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B13" s="22"/>
+      <c r="B13" s="24"/>
       <c r="C13" s="2" t="s">
         <v>17</v>
       </c>
@@ -1956,7 +2012,7 @@
       <c r="E13" s="2"/>
     </row>
     <row r="14" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B14" s="22"/>
+      <c r="B14" s="24"/>
       <c r="C14" s="2" t="s">
         <v>85</v>
       </c>
@@ -1964,7 +2020,7 @@
       <c r="E14" s="2"/>
     </row>
     <row r="15" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B15" s="22"/>
+      <c r="B15" s="24"/>
       <c r="C15" s="2" t="s">
         <v>14</v>
       </c>
@@ -1976,7 +2032,7 @@
       </c>
     </row>
     <row r="16" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B16" s="22"/>
+      <c r="B16" s="24"/>
       <c r="C16" s="17" t="s">
         <v>51</v>
       </c>
@@ -1984,7 +2040,7 @@
       <c r="E16" s="2"/>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B17" s="22"/>
+      <c r="B17" s="24"/>
       <c r="C17" s="2" t="s">
         <v>43</v>
       </c>
@@ -1992,7 +2048,7 @@
       <c r="E17" s="2"/>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B18" s="22" t="s">
+      <c r="B18" s="24" t="s">
         <v>18</v>
       </c>
       <c r="C18" s="2" t="s">
@@ -2004,7 +2060,7 @@
       <c r="E18" s="2"/>
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B19" s="22"/>
+      <c r="B19" s="24"/>
       <c r="C19" s="2" t="s">
         <v>20</v>
       </c>
@@ -2014,7 +2070,7 @@
       <c r="E19" s="2"/>
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B20" s="22"/>
+      <c r="B20" s="24"/>
       <c r="C20" s="2" t="s">
         <v>21</v>
       </c>
@@ -2024,7 +2080,7 @@
       <c r="E20" s="2"/>
     </row>
     <row r="21" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B21" s="22" t="s">
+      <c r="B21" s="24" t="s">
         <v>24</v>
       </c>
       <c r="C21" s="2" t="s">
@@ -2038,7 +2094,7 @@
       </c>
     </row>
     <row r="22" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B22" s="22"/>
+      <c r="B22" s="24"/>
       <c r="C22" s="2" t="s">
         <v>44</v>
       </c>
@@ -2050,7 +2106,7 @@
       </c>
     </row>
     <row r="23" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B23" s="22"/>
+      <c r="B23" s="24"/>
       <c r="C23" s="2" t="s">
         <v>23</v>
       </c>
@@ -2060,7 +2116,7 @@
       <c r="E23" s="2"/>
     </row>
     <row r="24" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B24" s="22" t="s">
+      <c r="B24" s="24" t="s">
         <v>25</v>
       </c>
       <c r="C24" s="2" t="s">
@@ -2074,7 +2130,7 @@
       </c>
     </row>
     <row r="25" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B25" s="22"/>
+      <c r="B25" s="24"/>
       <c r="C25" s="2" t="s">
         <v>45</v>
       </c>
@@ -2086,7 +2142,7 @@
       </c>
     </row>
     <row r="26" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B26" s="22"/>
+      <c r="B26" s="24"/>
       <c r="C26" s="2" t="s">
         <v>27</v>
       </c>
@@ -2096,7 +2152,7 @@
       <c r="E26" s="2"/>
     </row>
     <row r="27" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B27" s="22" t="s">
+      <c r="B27" s="24" t="s">
         <v>28</v>
       </c>
       <c r="C27" s="2" t="s">
@@ -2108,7 +2164,7 @@
       <c r="E27" s="2"/>
     </row>
     <row r="28" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B28" s="22"/>
+      <c r="B28" s="24"/>
       <c r="C28" s="2" t="s">
         <v>46</v>
       </c>
@@ -2116,7 +2172,7 @@
       <c r="E28" s="2"/>
     </row>
     <row r="29" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B29" s="22"/>
+      <c r="B29" s="24"/>
       <c r="C29" s="2" t="s">
         <v>30</v>
       </c>
@@ -2126,7 +2182,7 @@
       <c r="E29" s="2"/>
     </row>
     <row r="30" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B30" s="22" t="s">
+      <c r="B30" s="24" t="s">
         <v>32</v>
       </c>
       <c r="C30" s="2" t="s">
@@ -2140,7 +2196,7 @@
       </c>
     </row>
     <row r="31" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B31" s="22"/>
+      <c r="B31" s="24"/>
       <c r="C31" s="2" t="s">
         <v>33</v>
       </c>
@@ -2152,7 +2208,7 @@
       </c>
     </row>
     <row r="32" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B32" s="22"/>
+      <c r="B32" s="24"/>
       <c r="C32" s="2" t="s">
         <v>47</v>
       </c>
@@ -2238,7 +2294,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:C13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
@@ -2303,7 +2359,7 @@
   <dimension ref="A1:H24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2797,4 +2853,59 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:B8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="78.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B2" s="22" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="3" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="4" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="5" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="6" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="7" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="8" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>106</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
filtros - lista de doencas
</commit_message>
<xml_diff>
--- a/Modulos de actividades.xlsx
+++ b/Modulos de actividades.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="60" windowWidth="20115" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="60" windowWidth="20115" windowHeight="8010" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="front-end" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="106">
   <si>
     <t>Modulos</t>
   </si>
@@ -333,6 +333,9 @@
   </si>
   <si>
     <t>Nas edicoes do admin o botao cancelar nao pode ser um  type="reset"</t>
+  </si>
+  <si>
+    <t>adicionar tooltips nos icones de editar, adicionar e apagar</t>
   </si>
 </sst>
 </file>
@@ -1872,7 +1875,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:F34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+    <sheetView topLeftCell="A11" workbookViewId="0">
       <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
@@ -2842,10 +2845,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:B8"/>
+  <dimension ref="B2:B9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2889,6 +2892,11 @@
         <v>104</v>
       </c>
     </row>
+    <row r="9" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>105</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>